<commit_message>
chinese version xlsx with id
</commit_message>
<xml_diff>
--- a/look/look/excel_ch_remake/electrical.xlsx
+++ b/look/look/excel_ch_remake/electrical.xlsx
@@ -34945,6 +34945,9 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="B2" s="0" t="s">
         <v>9</v>
       </c>
@@ -34968,6 +34971,9 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="n">
+        <v>2</v>
+      </c>
       <c r="B3" s="0" t="s">
         <v>16</v>
       </c>
@@ -34991,6 +34997,9 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="n">
+        <v>3</v>
+      </c>
       <c r="B4" s="0" t="s">
         <v>9</v>
       </c>
@@ -35014,6 +35023,9 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="n">
+        <v>4</v>
+      </c>
       <c r="B5" s="0" t="s">
         <v>29</v>
       </c>
@@ -35037,6 +35049,9 @@
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="n">
+        <v>5</v>
+      </c>
       <c r="B6" s="0" t="s">
         <v>36</v>
       </c>
@@ -35060,6 +35075,9 @@
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="n">
+        <v>6</v>
+      </c>
       <c r="B7" s="0" t="s">
         <v>43</v>
       </c>
@@ -35083,6 +35101,9 @@
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="n">
+        <v>7</v>
+      </c>
       <c r="B8" s="0" t="s">
         <v>43</v>
       </c>
@@ -35106,6 +35127,9 @@
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="n">
+        <v>8</v>
+      </c>
       <c r="B9" s="0" t="s">
         <v>56</v>
       </c>
@@ -35129,6 +35153,9 @@
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="n">
+        <v>9</v>
+      </c>
       <c r="B10" s="0" t="s">
         <v>29</v>
       </c>
@@ -35152,6 +35179,9 @@
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="n">
+        <v>10</v>
+      </c>
       <c r="B11" s="0" t="s">
         <v>68</v>
       </c>
@@ -35175,6 +35205,9 @@
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="n">
+        <v>11</v>
+      </c>
       <c r="B12" s="0" t="s">
         <v>29</v>
       </c>
@@ -35198,6 +35231,9 @@
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="n">
+        <v>12</v>
+      </c>
       <c r="B13" s="0" t="s">
         <v>68</v>
       </c>
@@ -35221,6 +35257,9 @@
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="n">
+        <v>13</v>
+      </c>
       <c r="B14" s="0" t="s">
         <v>86</v>
       </c>
@@ -35244,6 +35283,9 @@
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="n">
+        <v>14</v>
+      </c>
       <c r="B15" s="0" t="s">
         <v>93</v>
       </c>
@@ -35267,6 +35309,9 @@
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="n">
+        <v>15</v>
+      </c>
       <c r="B16" s="0" t="s">
         <v>36</v>
       </c>
@@ -35290,6 +35335,9 @@
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="n">
+        <v>16</v>
+      </c>
       <c r="B17" s="0" t="s">
         <v>93</v>
       </c>
@@ -35313,6 +35361,9 @@
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="n">
+        <v>17</v>
+      </c>
       <c r="B18" s="0" t="s">
         <v>93</v>
       </c>
@@ -35336,6 +35387,9 @@
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="n">
+        <v>18</v>
+      </c>
       <c r="B19" s="0" t="s">
         <v>118</v>
       </c>
@@ -35359,6 +35413,9 @@
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="n">
+        <v>19</v>
+      </c>
       <c r="B20" s="0" t="s">
         <v>125</v>
       </c>
@@ -35382,6 +35439,9 @@
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="n">
+        <v>20</v>
+      </c>
       <c r="B21" s="0" t="s">
         <v>36</v>
       </c>
@@ -35405,6 +35465,9 @@
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="n">
+        <v>21</v>
+      </c>
       <c r="B22" s="0" t="s">
         <v>68</v>
       </c>
@@ -35428,6 +35491,9 @@
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="n">
+        <v>22</v>
+      </c>
       <c r="B23" s="0" t="s">
         <v>125</v>
       </c>
@@ -35451,6 +35517,9 @@
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="n">
+        <v>23</v>
+      </c>
       <c r="B24" s="0" t="s">
         <v>149</v>
       </c>
@@ -35474,6 +35543,9 @@
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="n">
+        <v>24</v>
+      </c>
       <c r="B25" s="0" t="s">
         <v>68</v>
       </c>
@@ -35497,6 +35569,9 @@
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="n">
+        <v>25</v>
+      </c>
       <c r="B26" s="0" t="s">
         <v>162</v>
       </c>
@@ -35520,6 +35595,9 @@
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="n">
+        <v>26</v>
+      </c>
       <c r="B27" s="0" t="s">
         <v>86</v>
       </c>
@@ -35543,6 +35621,9 @@
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="n">
+        <v>27</v>
+      </c>
       <c r="B28" s="0" t="s">
         <v>93</v>
       </c>
@@ -35566,6 +35647,9 @@
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="n">
+        <v>28</v>
+      </c>
       <c r="B29" s="0" t="s">
         <v>93</v>
       </c>
@@ -35589,6 +35673,9 @@
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="n">
+        <v>29</v>
+      </c>
       <c r="B30" s="0" t="s">
         <v>56</v>
       </c>
@@ -35612,6 +35699,9 @@
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0" t="n">
+        <v>30</v>
+      </c>
       <c r="B31" s="0" t="s">
         <v>118</v>
       </c>
@@ -35635,6 +35725,9 @@
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0" t="n">
+        <v>31</v>
+      </c>
       <c r="B32" s="0" t="s">
         <v>125</v>
       </c>
@@ -35658,6 +35751,9 @@
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0" t="n">
+        <v>32</v>
+      </c>
       <c r="B33" s="0" t="s">
         <v>149</v>
       </c>
@@ -35681,6 +35777,9 @@
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0" t="n">
+        <v>33</v>
+      </c>
       <c r="B34" s="0" t="s">
         <v>56</v>
       </c>
@@ -35704,6 +35803,9 @@
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="0" t="n">
+        <v>34</v>
+      </c>
       <c r="B35" s="0" t="s">
         <v>214</v>
       </c>
@@ -35727,6 +35829,9 @@
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="0" t="n">
+        <v>35</v>
+      </c>
       <c r="B36" s="0" t="s">
         <v>220</v>
       </c>
@@ -35750,6 +35855,9 @@
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="0" t="n">
+        <v>36</v>
+      </c>
       <c r="B37" s="0" t="s">
         <v>86</v>
       </c>
@@ -35773,6 +35881,9 @@
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="0" t="n">
+        <v>37</v>
+      </c>
       <c r="B38" s="0" t="s">
         <v>68</v>
       </c>
@@ -35796,6 +35907,9 @@
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="0" t="n">
+        <v>38</v>
+      </c>
       <c r="B39" s="0" t="s">
         <v>86</v>
       </c>
@@ -35819,6 +35933,9 @@
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="0" t="n">
+        <v>39</v>
+      </c>
       <c r="B40" s="0" t="s">
         <v>244</v>
       </c>
@@ -35842,6 +35959,9 @@
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="0" t="n">
+        <v>40</v>
+      </c>
       <c r="B41" s="0" t="s">
         <v>250</v>
       </c>
@@ -35865,6 +35985,9 @@
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="0" t="n">
+        <v>41</v>
+      </c>
       <c r="B42" s="0" t="s">
         <v>9</v>
       </c>
@@ -35888,6 +36011,9 @@
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="0" t="n">
+        <v>42</v>
+      </c>
       <c r="B43" s="0" t="s">
         <v>262</v>
       </c>
@@ -35911,6 +36037,9 @@
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="0" t="n">
+        <v>43</v>
+      </c>
       <c r="B44" s="0" t="s">
         <v>268</v>
       </c>
@@ -35934,6 +36063,9 @@
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="0" t="n">
+        <v>44</v>
+      </c>
       <c r="B45" s="0" t="s">
         <v>93</v>
       </c>
@@ -35957,6 +36089,9 @@
       </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="0" t="n">
+        <v>45</v>
+      </c>
       <c r="B46" s="0" t="s">
         <v>86</v>
       </c>
@@ -35980,6 +36115,9 @@
       </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="0" t="n">
+        <v>46</v>
+      </c>
       <c r="B47" s="0" t="s">
         <v>125</v>
       </c>
@@ -36003,6 +36141,9 @@
       </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="0" t="n">
+        <v>47</v>
+      </c>
       <c r="B48" s="0" t="s">
         <v>29</v>
       </c>
@@ -36026,6 +36167,9 @@
       </c>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="0" t="n">
+        <v>48</v>
+      </c>
       <c r="B49" s="0" t="s">
         <v>298</v>
       </c>
@@ -36049,6 +36193,9 @@
       </c>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="0" t="n">
+        <v>49</v>
+      </c>
       <c r="B50" s="0" t="s">
         <v>68</v>
       </c>
@@ -36072,6 +36219,9 @@
       </c>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="0" t="n">
+        <v>50</v>
+      </c>
       <c r="B51" s="0" t="s">
         <v>125</v>
       </c>
@@ -36095,6 +36245,9 @@
       </c>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="0" t="n">
+        <v>51</v>
+      </c>
       <c r="B52" s="0" t="s">
         <v>162</v>
       </c>
@@ -36118,6 +36271,9 @@
       </c>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="0" t="n">
+        <v>52</v>
+      </c>
       <c r="B53" s="0" t="s">
         <v>118</v>
       </c>
@@ -36141,6 +36297,9 @@
       </c>
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="0" t="n">
+        <v>53</v>
+      </c>
       <c r="B54" s="0" t="s">
         <v>325</v>
       </c>
@@ -36164,6 +36323,9 @@
       </c>
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="0" t="n">
+        <v>54</v>
+      </c>
       <c r="B55" s="0" t="s">
         <v>93</v>
       </c>
@@ -36187,6 +36349,9 @@
       </c>
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="0" t="n">
+        <v>55</v>
+      </c>
       <c r="B56" s="0" t="s">
         <v>262</v>
       </c>
@@ -36210,6 +36375,9 @@
       </c>
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="0" t="n">
+        <v>56</v>
+      </c>
       <c r="B57" s="0" t="s">
         <v>68</v>
       </c>
@@ -36233,6 +36401,9 @@
       </c>
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="0" t="n">
+        <v>57</v>
+      </c>
       <c r="B58" s="0" t="s">
         <v>298</v>
       </c>
@@ -36256,6 +36427,9 @@
       </c>
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="0" t="n">
+        <v>58</v>
+      </c>
       <c r="B59" s="0" t="s">
         <v>325</v>
       </c>
@@ -36279,6 +36453,9 @@
       </c>
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="0" t="n">
+        <v>59</v>
+      </c>
       <c r="B60" s="0" t="s">
         <v>360</v>
       </c>
@@ -36302,6 +36479,9 @@
       </c>
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="0" t="n">
+        <v>60</v>
+      </c>
       <c r="B61" s="0" t="s">
         <v>118</v>
       </c>
@@ -36325,6 +36505,9 @@
       </c>
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="0" t="n">
+        <v>61</v>
+      </c>
       <c r="B62" s="0" t="s">
         <v>86</v>
       </c>
@@ -36348,6 +36531,9 @@
       </c>
     </row>
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="0" t="n">
+        <v>62</v>
+      </c>
       <c r="B63" s="0" t="s">
         <v>56</v>
       </c>
@@ -36371,6 +36557,9 @@
       </c>
     </row>
     <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="0" t="n">
+        <v>63</v>
+      </c>
       <c r="B64" s="0" t="s">
         <v>93</v>
       </c>
@@ -36394,6 +36583,9 @@
       </c>
     </row>
     <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="0" t="n">
+        <v>64</v>
+      </c>
       <c r="B65" s="0" t="s">
         <v>125</v>
       </c>
@@ -36417,6 +36609,9 @@
       </c>
     </row>
     <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="0" t="n">
+        <v>65</v>
+      </c>
       <c r="B66" s="0" t="s">
         <v>93</v>
       </c>
@@ -36440,6 +36635,9 @@
       </c>
     </row>
     <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="0" t="n">
+        <v>66</v>
+      </c>
       <c r="B67" s="0" t="s">
         <v>118</v>
       </c>
@@ -36463,6 +36661,9 @@
       </c>
     </row>
     <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="0" t="n">
+        <v>67</v>
+      </c>
       <c r="B68" s="0" t="s">
         <v>125</v>
       </c>
@@ -36486,6 +36687,9 @@
       </c>
     </row>
     <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="0" t="n">
+        <v>68</v>
+      </c>
       <c r="B69" s="0" t="s">
         <v>214</v>
       </c>
@@ -36509,6 +36713,9 @@
       </c>
     </row>
     <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="0" t="n">
+        <v>69</v>
+      </c>
       <c r="B70" s="0" t="s">
         <v>29</v>
       </c>
@@ -36532,6 +36739,9 @@
       </c>
     </row>
     <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="0" t="n">
+        <v>70</v>
+      </c>
       <c r="B71" s="0" t="s">
         <v>56</v>
       </c>
@@ -36555,6 +36765,9 @@
       </c>
     </row>
     <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A72" s="0" t="n">
+        <v>71</v>
+      </c>
       <c r="B72" s="0" t="s">
         <v>118</v>
       </c>
@@ -36578,6 +36791,9 @@
       </c>
     </row>
     <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A73" s="0" t="n">
+        <v>72</v>
+      </c>
       <c r="B73" s="0" t="s">
         <v>118</v>
       </c>
@@ -36601,6 +36817,9 @@
       </c>
     </row>
     <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A74" s="0" t="n">
+        <v>73</v>
+      </c>
       <c r="B74" s="0" t="s">
         <v>93</v>
       </c>
@@ -36624,6 +36843,9 @@
       </c>
     </row>
     <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A75" s="0" t="n">
+        <v>74</v>
+      </c>
       <c r="B75" s="0" t="s">
         <v>149</v>
       </c>
@@ -36647,6 +36869,9 @@
       </c>
     </row>
     <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="0" t="n">
+        <v>75</v>
+      </c>
       <c r="B76" s="0" t="s">
         <v>68</v>
       </c>
@@ -36670,6 +36895,9 @@
       </c>
     </row>
     <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A77" s="0" t="n">
+        <v>76</v>
+      </c>
       <c r="B77" s="0" t="s">
         <v>86</v>
       </c>
@@ -36693,6 +36921,9 @@
       </c>
     </row>
     <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="0" t="n">
+        <v>77</v>
+      </c>
       <c r="B78" s="0" t="s">
         <v>93</v>
       </c>
@@ -36716,6 +36947,9 @@
       </c>
     </row>
     <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A79" s="0" t="n">
+        <v>78</v>
+      </c>
       <c r="B79" s="0" t="s">
         <v>464</v>
       </c>
@@ -36739,6 +36973,9 @@
       </c>
     </row>
     <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A80" s="0" t="n">
+        <v>79</v>
+      </c>
       <c r="B80" s="0" t="s">
         <v>470</v>
       </c>
@@ -36762,6 +36999,9 @@
       </c>
     </row>
     <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A81" s="0" t="n">
+        <v>80</v>
+      </c>
       <c r="B81" s="0" t="s">
         <v>86</v>
       </c>
@@ -36785,6 +37025,9 @@
       </c>
     </row>
     <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A82" s="0" t="n">
+        <v>81</v>
+      </c>
       <c r="B82" s="0" t="s">
         <v>149</v>
       </c>
@@ -36808,6 +37051,9 @@
       </c>
     </row>
     <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A83" s="0" t="n">
+        <v>82</v>
+      </c>
       <c r="B83" s="0" t="s">
         <v>86</v>
       </c>
@@ -36831,6 +37077,9 @@
       </c>
     </row>
     <row r="84" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A84" s="0" t="n">
+        <v>83</v>
+      </c>
       <c r="B84" s="0" t="s">
         <v>29</v>
       </c>
@@ -36854,6 +37103,9 @@
       </c>
     </row>
     <row r="85" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A85" s="0" t="n">
+        <v>84</v>
+      </c>
       <c r="B85" s="0" t="s">
         <v>499</v>
       </c>
@@ -36877,6 +37129,9 @@
       </c>
     </row>
     <row r="86" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A86" s="0" t="n">
+        <v>85</v>
+      </c>
       <c r="B86" s="0" t="s">
         <v>149</v>
       </c>
@@ -36900,6 +37155,9 @@
       </c>
     </row>
     <row r="87" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A87" s="0" t="n">
+        <v>86</v>
+      </c>
       <c r="B87" s="0" t="s">
         <v>244</v>
       </c>
@@ -36923,6 +37181,9 @@
       </c>
     </row>
     <row r="88" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A88" s="0" t="n">
+        <v>87</v>
+      </c>
       <c r="B88" s="0" t="s">
         <v>118</v>
       </c>
@@ -36946,6 +37207,9 @@
       </c>
     </row>
     <row r="89" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A89" s="0" t="n">
+        <v>88</v>
+      </c>
       <c r="B89" s="0" t="s">
         <v>149</v>
       </c>
@@ -36969,6 +37233,9 @@
       </c>
     </row>
     <row r="90" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A90" s="0" t="n">
+        <v>89</v>
+      </c>
       <c r="B90" s="0" t="s">
         <v>86</v>
       </c>
@@ -36992,6 +37259,9 @@
       </c>
     </row>
     <row r="91" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A91" s="0" t="n">
+        <v>90</v>
+      </c>
       <c r="B91" s="0" t="s">
         <v>470</v>
       </c>
@@ -37015,6 +37285,9 @@
       </c>
     </row>
     <row r="92" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A92" s="0" t="n">
+        <v>91</v>
+      </c>
       <c r="B92" s="0" t="s">
         <v>86</v>
       </c>
@@ -37038,6 +37311,9 @@
       </c>
     </row>
     <row r="93" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A93" s="0" t="n">
+        <v>92</v>
+      </c>
       <c r="B93" s="0" t="s">
         <v>149</v>
       </c>
@@ -37061,6 +37337,9 @@
       </c>
     </row>
     <row r="94" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A94" s="0" t="n">
+        <v>93</v>
+      </c>
       <c r="B94" s="0" t="s">
         <v>149</v>
       </c>
@@ -37084,6 +37363,9 @@
       </c>
     </row>
     <row r="95" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A95" s="0" t="n">
+        <v>94</v>
+      </c>
       <c r="B95" s="0" t="s">
         <v>86</v>
       </c>
@@ -37107,6 +37389,9 @@
       </c>
     </row>
     <row r="96" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A96" s="0" t="n">
+        <v>95</v>
+      </c>
       <c r="B96" s="0" t="s">
         <v>93</v>
       </c>
@@ -37130,6 +37415,9 @@
       </c>
     </row>
     <row r="97" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A97" s="0" t="n">
+        <v>96</v>
+      </c>
       <c r="B97" s="0" t="s">
         <v>149</v>
       </c>
@@ -37153,6 +37441,9 @@
       </c>
     </row>
     <row r="98" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A98" s="0" t="n">
+        <v>97</v>
+      </c>
       <c r="B98" s="0" t="s">
         <v>220</v>
       </c>
@@ -37176,6 +37467,9 @@
       </c>
     </row>
     <row r="99" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A99" s="0" t="n">
+        <v>98</v>
+      </c>
       <c r="B99" s="0" t="s">
         <v>29</v>
       </c>
@@ -37199,6 +37493,9 @@
       </c>
     </row>
     <row r="100" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A100" s="0" t="n">
+        <v>99</v>
+      </c>
       <c r="B100" s="0" t="s">
         <v>29</v>
       </c>
@@ -37222,6 +37519,9 @@
       </c>
     </row>
     <row r="101" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A101" s="0" t="n">
+        <v>100</v>
+      </c>
       <c r="B101" s="0" t="s">
         <v>93</v>
       </c>
@@ -37245,6 +37545,9 @@
       </c>
     </row>
     <row r="102" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A102" s="0" t="n">
+        <v>101</v>
+      </c>
       <c r="B102" s="0" t="s">
         <v>590</v>
       </c>
@@ -37268,6 +37571,9 @@
       </c>
     </row>
     <row r="103" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A103" s="0" t="n">
+        <v>102</v>
+      </c>
       <c r="B103" s="0" t="s">
         <v>118</v>
       </c>
@@ -37291,6 +37597,9 @@
       </c>
     </row>
     <row r="104" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A104" s="0" t="n">
+        <v>103</v>
+      </c>
       <c r="B104" s="0" t="s">
         <v>262</v>
       </c>
@@ -37314,6 +37623,9 @@
       </c>
     </row>
     <row r="105" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A105" s="0" t="n">
+        <v>104</v>
+      </c>
       <c r="B105" s="0" t="s">
         <v>149</v>
       </c>
@@ -37337,6 +37649,9 @@
       </c>
     </row>
     <row r="106" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A106" s="0" t="n">
+        <v>105</v>
+      </c>
       <c r="B106" s="0" t="s">
         <v>43</v>
       </c>
@@ -37360,6 +37675,9 @@
       </c>
     </row>
     <row r="107" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A107" s="0" t="n">
+        <v>106</v>
+      </c>
       <c r="B107" s="0" t="s">
         <v>118</v>
       </c>
@@ -37383,6 +37701,9 @@
       </c>
     </row>
     <row r="108" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A108" s="0" t="n">
+        <v>107</v>
+      </c>
       <c r="B108" s="0" t="s">
         <v>118</v>
       </c>
@@ -37406,6 +37727,9 @@
       </c>
     </row>
     <row r="109" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A109" s="0" t="n">
+        <v>108</v>
+      </c>
       <c r="B109" s="0" t="s">
         <v>298</v>
       </c>
@@ -37429,6 +37753,9 @@
       </c>
     </row>
     <row r="110" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A110" s="0" t="n">
+        <v>109</v>
+      </c>
       <c r="B110" s="0" t="s">
         <v>93</v>
       </c>
@@ -37452,6 +37779,9 @@
       </c>
     </row>
     <row r="111" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A111" s="0" t="n">
+        <v>110</v>
+      </c>
       <c r="B111" s="0" t="s">
         <v>29</v>
       </c>
@@ -37475,6 +37805,9 @@
       </c>
     </row>
     <row r="112" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A112" s="0" t="n">
+        <v>111</v>
+      </c>
       <c r="B112" s="0" t="s">
         <v>93</v>
       </c>
@@ -37498,6 +37831,9 @@
       </c>
     </row>
     <row r="113" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A113" s="0" t="n">
+        <v>112</v>
+      </c>
       <c r="B113" s="0" t="s">
         <v>651</v>
       </c>
@@ -37521,6 +37857,9 @@
       </c>
     </row>
     <row r="114" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A114" s="0" t="n">
+        <v>113</v>
+      </c>
       <c r="B114" s="0" t="s">
         <v>470</v>
       </c>
@@ -37544,6 +37883,9 @@
       </c>
     </row>
     <row r="115" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A115" s="0" t="n">
+        <v>114</v>
+      </c>
       <c r="B115" s="0" t="s">
         <v>9</v>
       </c>
@@ -37567,6 +37909,9 @@
       </c>
     </row>
     <row r="116" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A116" s="0" t="n">
+        <v>115</v>
+      </c>
       <c r="B116" s="0" t="s">
         <v>86</v>
       </c>
@@ -37590,6 +37935,9 @@
       </c>
     </row>
     <row r="117" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A117" s="0" t="n">
+        <v>116</v>
+      </c>
       <c r="B117" s="0" t="s">
         <v>464</v>
       </c>
@@ -37613,6 +37961,9 @@
       </c>
     </row>
     <row r="118" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A118" s="0" t="n">
+        <v>117</v>
+      </c>
       <c r="B118" s="0" t="s">
         <v>118</v>
       </c>
@@ -37636,6 +37987,9 @@
       </c>
     </row>
     <row r="119" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A119" s="0" t="n">
+        <v>118</v>
+      </c>
       <c r="B119" s="0" t="s">
         <v>125</v>
       </c>
@@ -37659,6 +38013,9 @@
       </c>
     </row>
     <row r="120" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A120" s="0" t="n">
+        <v>119</v>
+      </c>
       <c r="B120" s="0" t="s">
         <v>298</v>
       </c>
@@ -37682,6 +38039,9 @@
       </c>
     </row>
     <row r="121" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A121" s="0" t="n">
+        <v>120</v>
+      </c>
       <c r="B121" s="0" t="s">
         <v>29</v>
       </c>
@@ -37705,6 +38065,9 @@
       </c>
     </row>
     <row r="122" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A122" s="0" t="n">
+        <v>121</v>
+      </c>
       <c r="B122" s="0" t="s">
         <v>56</v>
       </c>
@@ -37728,6 +38091,9 @@
       </c>
     </row>
     <row r="123" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A123" s="0" t="n">
+        <v>122</v>
+      </c>
       <c r="B123" s="0" t="s">
         <v>68</v>
       </c>
@@ -37751,6 +38117,9 @@
       </c>
     </row>
     <row r="124" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A124" s="0" t="n">
+        <v>123</v>
+      </c>
       <c r="B124" s="0" t="s">
         <v>214</v>
       </c>
@@ -37774,6 +38143,9 @@
       </c>
     </row>
     <row r="125" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A125" s="0" t="n">
+        <v>124</v>
+      </c>
       <c r="B125" s="0" t="s">
         <v>29</v>
       </c>
@@ -37797,6 +38169,9 @@
       </c>
     </row>
     <row r="126" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A126" s="0" t="n">
+        <v>125</v>
+      </c>
       <c r="B126" s="0" t="s">
         <v>9</v>
       </c>
@@ -37820,6 +38195,9 @@
       </c>
     </row>
     <row r="127" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A127" s="0" t="n">
+        <v>126</v>
+      </c>
       <c r="B127" s="0" t="s">
         <v>16</v>
       </c>
@@ -37843,6 +38221,9 @@
       </c>
     </row>
     <row r="128" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A128" s="0" t="n">
+        <v>127</v>
+      </c>
       <c r="B128" s="0" t="s">
         <v>464</v>
       </c>
@@ -37866,6 +38247,9 @@
       </c>
     </row>
     <row r="129" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A129" s="0" t="n">
+        <v>128</v>
+      </c>
       <c r="B129" s="0" t="s">
         <v>737</v>
       </c>
@@ -37889,6 +38273,9 @@
       </c>
     </row>
     <row r="130" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A130" s="0" t="n">
+        <v>129</v>
+      </c>
       <c r="B130" s="0" t="s">
         <v>93</v>
       </c>
@@ -37912,6 +38299,9 @@
       </c>
     </row>
     <row r="131" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A131" s="0" t="n">
+        <v>130</v>
+      </c>
       <c r="B131" s="0" t="s">
         <v>244</v>
       </c>
@@ -37935,6 +38325,9 @@
       </c>
     </row>
     <row r="132" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A132" s="0" t="n">
+        <v>131</v>
+      </c>
       <c r="B132" s="0" t="s">
         <v>118</v>
       </c>
@@ -37958,6 +38351,9 @@
       </c>
     </row>
     <row r="133" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A133" s="0" t="n">
+        <v>132</v>
+      </c>
       <c r="B133" s="0" t="s">
         <v>149</v>
       </c>
@@ -37981,6 +38377,9 @@
       </c>
     </row>
     <row r="134" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A134" s="0" t="n">
+        <v>133</v>
+      </c>
       <c r="B134" s="0" t="s">
         <v>9</v>
       </c>
@@ -38004,6 +38403,9 @@
       </c>
     </row>
     <row r="135" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A135" s="0" t="n">
+        <v>134</v>
+      </c>
       <c r="B135" s="0" t="s">
         <v>162</v>
       </c>
@@ -38027,6 +38429,9 @@
       </c>
     </row>
     <row r="136" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A136" s="0" t="n">
+        <v>135</v>
+      </c>
       <c r="B136" s="0" t="s">
         <v>325</v>
       </c>
@@ -38050,6 +38455,9 @@
       </c>
     </row>
     <row r="137" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A137" s="0" t="n">
+        <v>136</v>
+      </c>
       <c r="B137" s="0" t="s">
         <v>86</v>
       </c>
@@ -38073,6 +38481,9 @@
       </c>
     </row>
     <row r="138" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A138" s="0" t="n">
+        <v>137</v>
+      </c>
       <c r="B138" s="0" t="s">
         <v>149</v>
       </c>
@@ -38096,6 +38507,9 @@
       </c>
     </row>
     <row r="139" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A139" s="0" t="n">
+        <v>138</v>
+      </c>
       <c r="B139" s="0" t="s">
         <v>86</v>
       </c>
@@ -38119,6 +38533,9 @@
       </c>
     </row>
     <row r="140" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A140" s="0" t="n">
+        <v>139</v>
+      </c>
       <c r="B140" s="0" t="s">
         <v>298</v>
       </c>
@@ -38142,6 +38559,9 @@
       </c>
     </row>
     <row r="141" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A141" s="0" t="n">
+        <v>140</v>
+      </c>
       <c r="B141" s="0" t="s">
         <v>149</v>
       </c>
@@ -38165,6 +38585,9 @@
       </c>
     </row>
     <row r="142" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A142" s="0" t="n">
+        <v>141</v>
+      </c>
       <c r="B142" s="0" t="s">
         <v>149</v>
       </c>
@@ -38188,6 +38611,9 @@
       </c>
     </row>
     <row r="143" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A143" s="0" t="n">
+        <v>142</v>
+      </c>
       <c r="B143" s="0" t="s">
         <v>464</v>
       </c>
@@ -38211,6 +38637,9 @@
       </c>
     </row>
     <row r="144" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A144" s="0" t="n">
+        <v>143</v>
+      </c>
       <c r="B144" s="0" t="s">
         <v>244</v>
       </c>
@@ -38234,6 +38663,9 @@
       </c>
     </row>
     <row r="145" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A145" s="0" t="n">
+        <v>144</v>
+      </c>
       <c r="B145" s="0" t="s">
         <v>737</v>
       </c>
@@ -38257,6 +38689,9 @@
       </c>
     </row>
     <row r="146" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A146" s="0" t="n">
+        <v>145</v>
+      </c>
       <c r="B146" s="0" t="s">
         <v>325</v>
       </c>
@@ -38280,6 +38715,9 @@
       </c>
     </row>
     <row r="147" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A147" s="0" t="n">
+        <v>146</v>
+      </c>
       <c r="B147" s="0" t="s">
         <v>149</v>
       </c>
@@ -38303,6 +38741,9 @@
       </c>
     </row>
     <row r="148" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A148" s="0" t="n">
+        <v>147</v>
+      </c>
       <c r="B148" s="0" t="s">
         <v>298</v>
       </c>
@@ -38326,6 +38767,9 @@
       </c>
     </row>
     <row r="149" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A149" s="0" t="n">
+        <v>148</v>
+      </c>
       <c r="B149" s="0" t="s">
         <v>149</v>
       </c>
@@ -38349,6 +38793,9 @@
       </c>
     </row>
     <row r="150" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A150" s="0" t="n">
+        <v>149</v>
+      </c>
       <c r="B150" s="0" t="s">
         <v>298</v>
       </c>
@@ -38372,6 +38819,9 @@
       </c>
     </row>
     <row r="151" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A151" s="0" t="n">
+        <v>150</v>
+      </c>
       <c r="B151" s="0" t="s">
         <v>298</v>
       </c>
@@ -38395,6 +38845,9 @@
       </c>
     </row>
     <row r="152" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A152" s="0" t="n">
+        <v>151</v>
+      </c>
       <c r="B152" s="0" t="s">
         <v>855</v>
       </c>
@@ -38418,6 +38871,9 @@
       </c>
     </row>
     <row r="153" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A153" s="0" t="n">
+        <v>152</v>
+      </c>
       <c r="B153" s="0" t="s">
         <v>651</v>
       </c>
@@ -38441,6 +38897,9 @@
       </c>
     </row>
     <row r="154" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A154" s="0" t="n">
+        <v>153</v>
+      </c>
       <c r="B154" s="0" t="s">
         <v>162</v>
       </c>
@@ -38464,6 +38923,9 @@
       </c>
     </row>
     <row r="155" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A155" s="0" t="n">
+        <v>154</v>
+      </c>
       <c r="B155" s="0" t="s">
         <v>86</v>
       </c>
@@ -38487,6 +38949,9 @@
       </c>
     </row>
     <row r="156" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A156" s="0" t="n">
+        <v>155</v>
+      </c>
       <c r="B156" s="0" t="s">
         <v>149</v>
       </c>
@@ -38510,6 +38975,9 @@
       </c>
     </row>
     <row r="157" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A157" s="0" t="n">
+        <v>156</v>
+      </c>
       <c r="B157" s="0" t="s">
         <v>737</v>
       </c>
@@ -38533,6 +39001,9 @@
       </c>
     </row>
     <row r="158" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A158" s="0" t="n">
+        <v>157</v>
+      </c>
       <c r="B158" s="0" t="s">
         <v>118</v>
       </c>
@@ -38556,6 +39027,9 @@
       </c>
     </row>
     <row r="159" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A159" s="0" t="n">
+        <v>158</v>
+      </c>
       <c r="B159" s="0" t="s">
         <v>149</v>
       </c>
@@ -38579,6 +39053,9 @@
       </c>
     </row>
     <row r="160" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A160" s="0" t="n">
+        <v>159</v>
+      </c>
       <c r="B160" s="0" t="s">
         <v>149</v>
       </c>
@@ -38602,6 +39079,9 @@
       </c>
     </row>
     <row r="161" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A161" s="0" t="n">
+        <v>160</v>
+      </c>
       <c r="B161" s="0" t="s">
         <v>162</v>
       </c>
@@ -38625,6 +39105,9 @@
       </c>
     </row>
     <row r="162" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A162" s="0" t="n">
+        <v>161</v>
+      </c>
       <c r="B162" s="0" t="s">
         <v>29</v>
       </c>
@@ -38648,6 +39131,9 @@
       </c>
     </row>
     <row r="163" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A163" s="0" t="n">
+        <v>162</v>
+      </c>
       <c r="B163" s="0" t="s">
         <v>298</v>
       </c>
@@ -38671,6 +39157,9 @@
       </c>
     </row>
     <row r="164" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A164" s="0" t="n">
+        <v>163</v>
+      </c>
       <c r="B164" s="0" t="s">
         <v>298</v>
       </c>
@@ -38694,6 +39183,9 @@
       </c>
     </row>
     <row r="165" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A165" s="0" t="n">
+        <v>164</v>
+      </c>
       <c r="B165" s="0" t="s">
         <v>93</v>
       </c>
@@ -38717,6 +39209,9 @@
       </c>
     </row>
     <row r="166" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A166" s="0" t="n">
+        <v>165</v>
+      </c>
       <c r="B166" s="0" t="s">
         <v>125</v>
       </c>
@@ -38740,6 +39235,9 @@
       </c>
     </row>
     <row r="167" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A167" s="0" t="n">
+        <v>166</v>
+      </c>
       <c r="B167" s="0" t="s">
         <v>298</v>
       </c>
@@ -38763,6 +39261,9 @@
       </c>
     </row>
     <row r="168" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A168" s="0" t="n">
+        <v>167</v>
+      </c>
       <c r="B168" s="0" t="s">
         <v>936</v>
       </c>
@@ -38786,6 +39287,9 @@
       </c>
     </row>
     <row r="169" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A169" s="0" t="n">
+        <v>168</v>
+      </c>
       <c r="B169" s="0" t="s">
         <v>149</v>
       </c>
@@ -38809,6 +39313,9 @@
       </c>
     </row>
     <row r="170" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A170" s="0" t="n">
+        <v>169</v>
+      </c>
       <c r="B170" s="0" t="s">
         <v>325</v>
       </c>
@@ -38832,6 +39339,9 @@
       </c>
     </row>
     <row r="171" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A171" s="0" t="n">
+        <v>170</v>
+      </c>
       <c r="B171" s="0" t="s">
         <v>298</v>
       </c>
@@ -38855,6 +39365,9 @@
       </c>
     </row>
     <row r="172" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A172" s="0" t="n">
+        <v>171</v>
+      </c>
       <c r="B172" s="0" t="s">
         <v>149</v>
       </c>
@@ -38878,6 +39391,9 @@
       </c>
     </row>
     <row r="173" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A173" s="0" t="n">
+        <v>172</v>
+      </c>
       <c r="B173" s="0" t="s">
         <v>93</v>
       </c>
@@ -38901,6 +39417,9 @@
       </c>
     </row>
     <row r="174" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A174" s="0" t="n">
+        <v>173</v>
+      </c>
       <c r="B174" s="0" t="s">
         <v>149</v>
       </c>
@@ -38924,6 +39443,9 @@
       </c>
     </row>
     <row r="175" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A175" s="0" t="n">
+        <v>174</v>
+      </c>
       <c r="B175" s="0" t="s">
         <v>325</v>
       </c>
@@ -38947,6 +39469,9 @@
       </c>
     </row>
     <row r="176" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A176" s="0" t="n">
+        <v>175</v>
+      </c>
       <c r="B176" s="0" t="s">
         <v>298</v>
       </c>
@@ -38970,6 +39495,9 @@
       </c>
     </row>
     <row r="177" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A177" s="0" t="n">
+        <v>176</v>
+      </c>
       <c r="B177" s="0" t="s">
         <v>93</v>
       </c>
@@ -38993,6 +39521,9 @@
       </c>
     </row>
     <row r="178" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A178" s="0" t="n">
+        <v>177</v>
+      </c>
       <c r="B178" s="0" t="s">
         <v>499</v>
       </c>
@@ -39016,6 +39547,9 @@
       </c>
     </row>
     <row r="179" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A179" s="0" t="n">
+        <v>178</v>
+      </c>
       <c r="B179" s="0" t="s">
         <v>118</v>
       </c>
@@ -39039,6 +39573,9 @@
       </c>
     </row>
     <row r="180" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A180" s="0" t="n">
+        <v>179</v>
+      </c>
       <c r="B180" s="0" t="s">
         <v>118</v>
       </c>
@@ -39062,6 +39599,9 @@
       </c>
     </row>
     <row r="181" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A181" s="0" t="n">
+        <v>180</v>
+      </c>
       <c r="B181" s="0" t="s">
         <v>464</v>
       </c>
@@ -39085,6 +39625,9 @@
       </c>
     </row>
     <row r="182" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A182" s="0" t="n">
+        <v>181</v>
+      </c>
       <c r="B182" s="0" t="s">
         <v>737</v>
       </c>
@@ -39108,6 +39651,9 @@
       </c>
     </row>
     <row r="183" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A183" s="0" t="n">
+        <v>182</v>
+      </c>
       <c r="B183" s="0" t="s">
         <v>737</v>
       </c>
@@ -39131,6 +39677,9 @@
       </c>
     </row>
     <row r="184" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A184" s="0" t="n">
+        <v>183</v>
+      </c>
       <c r="B184" s="0" t="s">
         <v>68</v>
       </c>
@@ -39154,6 +39703,9 @@
       </c>
     </row>
     <row r="185" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A185" s="0" t="n">
+        <v>184</v>
+      </c>
       <c r="B185" s="0" t="s">
         <v>149</v>
       </c>
@@ -39177,6 +39729,9 @@
       </c>
     </row>
     <row r="186" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A186" s="0" t="n">
+        <v>185</v>
+      </c>
       <c r="B186" s="0" t="s">
         <v>149</v>
       </c>
@@ -39200,6 +39755,9 @@
       </c>
     </row>
     <row r="187" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A187" s="0" t="n">
+        <v>186</v>
+      </c>
       <c r="B187" s="0" t="s">
         <v>118</v>
       </c>
@@ -39223,6 +39781,9 @@
       </c>
     </row>
     <row r="188" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A188" s="0" t="n">
+        <v>187</v>
+      </c>
       <c r="B188" s="0" t="s">
         <v>93</v>
       </c>
@@ -39246,6 +39807,9 @@
       </c>
     </row>
     <row r="189" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A189" s="0" t="n">
+        <v>188</v>
+      </c>
       <c r="B189" s="0" t="s">
         <v>118</v>
       </c>
@@ -39269,6 +39833,9 @@
       </c>
     </row>
     <row r="190" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A190" s="0" t="n">
+        <v>189</v>
+      </c>
       <c r="B190" s="0" t="s">
         <v>244</v>
       </c>
@@ -39292,6 +39859,9 @@
       </c>
     </row>
     <row r="191" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A191" s="0" t="n">
+        <v>190</v>
+      </c>
       <c r="B191" s="0" t="s">
         <v>149</v>
       </c>
@@ -39315,6 +39885,9 @@
       </c>
     </row>
     <row r="192" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A192" s="0" t="n">
+        <v>191</v>
+      </c>
       <c r="B192" s="0" t="s">
         <v>149</v>
       </c>
@@ -39338,6 +39911,9 @@
       </c>
     </row>
     <row r="193" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A193" s="0" t="n">
+        <v>192</v>
+      </c>
       <c r="B193" s="0" t="s">
         <v>118</v>
       </c>
@@ -39358,6 +39934,9 @@
       </c>
     </row>
     <row r="194" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A194" s="0" t="n">
+        <v>193</v>
+      </c>
       <c r="B194" s="0" t="s">
         <v>118</v>
       </c>
@@ -39381,6 +39960,9 @@
       </c>
     </row>
     <row r="195" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A195" s="0" t="n">
+        <v>194</v>
+      </c>
       <c r="B195" s="0" t="s">
         <v>118</v>
       </c>
@@ -39404,6 +39986,9 @@
       </c>
     </row>
     <row r="196" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A196" s="0" t="n">
+        <v>195</v>
+      </c>
       <c r="B196" s="0" t="s">
         <v>86</v>
       </c>
@@ -39427,6 +40012,9 @@
       </c>
     </row>
     <row r="197" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A197" s="0" t="n">
+        <v>196</v>
+      </c>
       <c r="B197" s="0" t="s">
         <v>360</v>
       </c>
@@ -39450,6 +40038,9 @@
       </c>
     </row>
     <row r="198" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A198" s="0" t="n">
+        <v>197</v>
+      </c>
       <c r="B198" s="0" t="s">
         <v>149</v>
       </c>
@@ -39473,6 +40064,9 @@
       </c>
     </row>
     <row r="199" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A199" s="0" t="n">
+        <v>198</v>
+      </c>
       <c r="B199" s="0" t="s">
         <v>86</v>
       </c>
@@ -39496,6 +40090,9 @@
       </c>
     </row>
     <row r="200" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A200" s="0" t="n">
+        <v>199</v>
+      </c>
       <c r="B200" s="0" t="s">
         <v>118</v>
       </c>
@@ -39519,6 +40116,9 @@
       </c>
     </row>
     <row r="201" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A201" s="0" t="n">
+        <v>200</v>
+      </c>
       <c r="B201" s="0" t="s">
         <v>737</v>
       </c>
@@ -39542,6 +40142,9 @@
       </c>
     </row>
     <row r="202" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A202" s="0" t="n">
+        <v>201</v>
+      </c>
       <c r="B202" s="0" t="s">
         <v>93</v>
       </c>
@@ -39565,6 +40168,9 @@
       </c>
     </row>
     <row r="203" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A203" s="0" t="n">
+        <v>202</v>
+      </c>
       <c r="B203" s="0" t="s">
         <v>118</v>
       </c>
@@ -39588,6 +40194,9 @@
       </c>
     </row>
     <row r="204" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A204" s="0" t="n">
+        <v>203</v>
+      </c>
       <c r="B204" s="0" t="s">
         <v>298</v>
       </c>
@@ -39611,6 +40220,9 @@
       </c>
     </row>
     <row r="205" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A205" s="0" t="n">
+        <v>204</v>
+      </c>
       <c r="B205" s="0" t="s">
         <v>149</v>
       </c>
@@ -39634,6 +40246,9 @@
       </c>
     </row>
     <row r="206" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A206" s="0" t="n">
+        <v>205</v>
+      </c>
       <c r="B206" s="0" t="s">
         <v>125</v>
       </c>
@@ -39657,6 +40272,9 @@
       </c>
     </row>
     <row r="207" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A207" s="0" t="n">
+        <v>206</v>
+      </c>
       <c r="B207" s="0" t="s">
         <v>149</v>
       </c>
@@ -39680,6 +40298,9 @@
       </c>
     </row>
     <row r="208" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A208" s="0" t="n">
+        <v>207</v>
+      </c>
       <c r="B208" s="0" t="s">
         <v>149</v>
       </c>
@@ -39703,6 +40324,9 @@
       </c>
     </row>
     <row r="209" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A209" s="0" t="n">
+        <v>208</v>
+      </c>
       <c r="B209" s="0" t="s">
         <v>325</v>
       </c>
@@ -39726,6 +40350,9 @@
       </c>
     </row>
     <row r="210" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A210" s="0" t="n">
+        <v>209</v>
+      </c>
       <c r="B210" s="0" t="s">
         <v>298</v>
       </c>
@@ -39749,6 +40376,9 @@
       </c>
     </row>
     <row r="211" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A211" s="0" t="n">
+        <v>210</v>
+      </c>
       <c r="B211" s="0" t="s">
         <v>125</v>
       </c>
@@ -39772,6 +40402,9 @@
       </c>
     </row>
     <row r="212" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A212" s="0" t="n">
+        <v>211</v>
+      </c>
       <c r="B212" s="0" t="s">
         <v>125</v>
       </c>
@@ -39795,6 +40428,9 @@
       </c>
     </row>
     <row r="213" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A213" s="0" t="n">
+        <v>212</v>
+      </c>
       <c r="B213" s="0" t="s">
         <v>590</v>
       </c>
@@ -39818,6 +40454,9 @@
       </c>
     </row>
     <row r="214" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A214" s="0" t="n">
+        <v>213</v>
+      </c>
       <c r="B214" s="0" t="s">
         <v>149</v>
       </c>
@@ -39841,6 +40480,9 @@
       </c>
     </row>
     <row r="215" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A215" s="0" t="n">
+        <v>214</v>
+      </c>
       <c r="B215" s="0" t="s">
         <v>737</v>
       </c>
@@ -39864,6 +40506,9 @@
       </c>
     </row>
     <row r="216" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A216" s="0" t="n">
+        <v>215</v>
+      </c>
       <c r="B216" s="0" t="s">
         <v>149</v>
       </c>
@@ -39887,6 +40532,9 @@
       </c>
     </row>
     <row r="217" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A217" s="0" t="n">
+        <v>216</v>
+      </c>
       <c r="B217" s="0" t="s">
         <v>56</v>
       </c>
@@ -39910,6 +40558,9 @@
       </c>
     </row>
     <row r="218" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A218" s="0" t="n">
+        <v>217</v>
+      </c>
       <c r="B218" s="0" t="s">
         <v>499</v>
       </c>
@@ -39933,6 +40584,9 @@
       </c>
     </row>
     <row r="219" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A219" s="0" t="n">
+        <v>218</v>
+      </c>
       <c r="B219" s="0" t="s">
         <v>86</v>
       </c>
@@ -39956,6 +40610,9 @@
       </c>
     </row>
     <row r="220" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A220" s="0" t="n">
+        <v>219</v>
+      </c>
       <c r="B220" s="0" t="s">
         <v>93</v>
       </c>
@@ -39979,6 +40636,9 @@
       </c>
     </row>
     <row r="221" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A221" s="0" t="n">
+        <v>220</v>
+      </c>
       <c r="B221" s="0" t="s">
         <v>149</v>
       </c>
@@ -40002,6 +40662,9 @@
       </c>
     </row>
     <row r="222" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A222" s="0" t="n">
+        <v>221</v>
+      </c>
       <c r="B222" s="0" t="s">
         <v>162</v>
       </c>
@@ -40025,6 +40688,9 @@
       </c>
     </row>
     <row r="223" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A223" s="0" t="n">
+        <v>222</v>
+      </c>
       <c r="B223" s="0" t="s">
         <v>118</v>
       </c>
@@ -40048,6 +40714,9 @@
       </c>
     </row>
     <row r="224" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A224" s="0" t="n">
+        <v>223</v>
+      </c>
       <c r="B224" s="0" t="s">
         <v>118</v>
       </c>
@@ -40071,6 +40740,9 @@
       </c>
     </row>
     <row r="225" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A225" s="0" t="n">
+        <v>224</v>
+      </c>
       <c r="B225" s="0" t="s">
         <v>86</v>
       </c>
@@ -40094,6 +40766,9 @@
       </c>
     </row>
     <row r="226" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A226" s="0" t="n">
+        <v>225</v>
+      </c>
       <c r="B226" s="0" t="s">
         <v>9</v>
       </c>
@@ -40117,6 +40792,9 @@
       </c>
     </row>
     <row r="227" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A227" s="0" t="n">
+        <v>226</v>
+      </c>
       <c r="B227" s="0" t="s">
         <v>118</v>
       </c>
@@ -40140,6 +40818,9 @@
       </c>
     </row>
     <row r="228" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A228" s="0" t="n">
+        <v>227</v>
+      </c>
       <c r="B228" s="0" t="s">
         <v>93</v>
       </c>
@@ -40163,6 +40844,9 @@
       </c>
     </row>
     <row r="229" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A229" s="0" t="n">
+        <v>228</v>
+      </c>
       <c r="B229" s="0" t="s">
         <v>43</v>
       </c>
@@ -40186,6 +40870,9 @@
       </c>
     </row>
     <row r="230" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A230" s="0" t="n">
+        <v>229</v>
+      </c>
       <c r="B230" s="0" t="s">
         <v>149</v>
       </c>
@@ -40209,6 +40896,9 @@
       </c>
     </row>
     <row r="231" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A231" s="0" t="n">
+        <v>230</v>
+      </c>
       <c r="B231" s="0" t="s">
         <v>29</v>
       </c>
@@ -40232,6 +40922,9 @@
       </c>
     </row>
     <row r="232" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A232" s="0" t="n">
+        <v>231</v>
+      </c>
       <c r="B232" s="0" t="s">
         <v>737</v>
       </c>
@@ -40255,6 +40948,9 @@
       </c>
     </row>
     <row r="233" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A233" s="0" t="n">
+        <v>232</v>
+      </c>
       <c r="B233" s="0" t="s">
         <v>86</v>
       </c>
@@ -40278,6 +40974,9 @@
       </c>
     </row>
     <row r="234" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A234" s="0" t="n">
+        <v>233</v>
+      </c>
       <c r="B234" s="0" t="s">
         <v>149</v>
       </c>
@@ -40301,6 +41000,9 @@
       </c>
     </row>
     <row r="235" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A235" s="0" t="n">
+        <v>234</v>
+      </c>
       <c r="B235" s="0" t="s">
         <v>86</v>
       </c>
@@ -40324,6 +41026,9 @@
       </c>
     </row>
     <row r="236" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A236" s="0" t="n">
+        <v>235</v>
+      </c>
       <c r="B236" s="0" t="s">
         <v>29</v>
       </c>
@@ -40347,6 +41052,9 @@
       </c>
     </row>
     <row r="237" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A237" s="0" t="n">
+        <v>236</v>
+      </c>
       <c r="B237" s="0" t="s">
         <v>936</v>
       </c>
@@ -40367,6 +41075,9 @@
       </c>
     </row>
     <row r="238" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A238" s="0" t="n">
+        <v>237</v>
+      </c>
       <c r="B238" s="0" t="s">
         <v>590</v>
       </c>
@@ -40390,6 +41101,9 @@
       </c>
     </row>
     <row r="239" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A239" s="0" t="n">
+        <v>238</v>
+      </c>
       <c r="B239" s="0" t="s">
         <v>68</v>
       </c>
@@ -40413,6 +41127,9 @@
       </c>
     </row>
     <row r="240" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A240" s="0" t="n">
+        <v>239</v>
+      </c>
       <c r="B240" s="0" t="s">
         <v>149</v>
       </c>
@@ -40436,6 +41153,9 @@
       </c>
     </row>
     <row r="241" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A241" s="0" t="n">
+        <v>240</v>
+      </c>
       <c r="B241" s="0" t="s">
         <v>125</v>
       </c>
@@ -40459,6 +41179,9 @@
       </c>
     </row>
     <row r="242" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A242" s="0" t="n">
+        <v>241</v>
+      </c>
       <c r="B242" s="0" t="s">
         <v>56</v>
       </c>
@@ -40482,6 +41205,9 @@
       </c>
     </row>
     <row r="243" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A243" s="0" t="n">
+        <v>242</v>
+      </c>
       <c r="B243" s="0" t="s">
         <v>93</v>
       </c>
@@ -40505,6 +41231,9 @@
       </c>
     </row>
     <row r="244" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A244" s="0" t="n">
+        <v>243</v>
+      </c>
       <c r="B244" s="0" t="s">
         <v>86</v>
       </c>
@@ -40528,6 +41257,9 @@
       </c>
     </row>
     <row r="245" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A245" s="0" t="n">
+        <v>244</v>
+      </c>
       <c r="B245" s="0" t="s">
         <v>149</v>
       </c>
@@ -40551,6 +41283,9 @@
       </c>
     </row>
     <row r="246" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A246" s="0" t="n">
+        <v>245</v>
+      </c>
       <c r="B246" s="0" t="s">
         <v>325</v>
       </c>
@@ -40574,6 +41309,9 @@
       </c>
     </row>
     <row r="247" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A247" s="0" t="n">
+        <v>246</v>
+      </c>
       <c r="B247" s="0" t="s">
         <v>149</v>
       </c>
@@ -40597,6 +41335,9 @@
       </c>
     </row>
     <row r="248" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A248" s="0" t="n">
+        <v>247</v>
+      </c>
       <c r="B248" s="0" t="s">
         <v>149</v>
       </c>
@@ -40620,6 +41361,9 @@
       </c>
     </row>
     <row r="249" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A249" s="0" t="n">
+        <v>248</v>
+      </c>
       <c r="B249" s="0" t="s">
         <v>118</v>
       </c>
@@ -40643,6 +41387,9 @@
       </c>
     </row>
     <row r="250" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A250" s="0" t="n">
+        <v>249</v>
+      </c>
       <c r="B250" s="0" t="s">
         <v>149</v>
       </c>
@@ -40666,6 +41413,9 @@
       </c>
     </row>
     <row r="251" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A251" s="0" t="n">
+        <v>250</v>
+      </c>
       <c r="B251" s="0" t="s">
         <v>149</v>
       </c>
@@ -40689,6 +41439,9 @@
       </c>
     </row>
     <row r="252" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A252" s="0" t="n">
+        <v>251</v>
+      </c>
       <c r="B252" s="0" t="s">
         <v>93</v>
       </c>
@@ -40712,6 +41465,9 @@
       </c>
     </row>
     <row r="253" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A253" s="0" t="n">
+        <v>252</v>
+      </c>
       <c r="B253" s="0" t="s">
         <v>855</v>
       </c>
@@ -40735,6 +41491,9 @@
       </c>
     </row>
     <row r="254" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A254" s="0" t="n">
+        <v>253</v>
+      </c>
       <c r="B254" s="0" t="s">
         <v>590</v>
       </c>
@@ -40758,6 +41517,9 @@
       </c>
     </row>
     <row r="255" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A255" s="0" t="n">
+        <v>254</v>
+      </c>
       <c r="B255" s="0" t="s">
         <v>737</v>
       </c>
@@ -40781,6 +41543,9 @@
       </c>
     </row>
     <row r="256" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A256" s="0" t="n">
+        <v>255</v>
+      </c>
       <c r="B256" s="0" t="s">
         <v>125</v>
       </c>
@@ -40804,6 +41569,9 @@
       </c>
     </row>
     <row r="257" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A257" s="0" t="n">
+        <v>256</v>
+      </c>
       <c r="B257" s="0" t="s">
         <v>118</v>
       </c>
@@ -40827,6 +41595,9 @@
       </c>
     </row>
     <row r="258" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A258" s="0" t="n">
+        <v>257</v>
+      </c>
       <c r="B258" s="0" t="s">
         <v>125</v>
       </c>
@@ -40850,6 +41621,9 @@
       </c>
     </row>
     <row r="259" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A259" s="0" t="n">
+        <v>258</v>
+      </c>
       <c r="B259" s="0" t="s">
         <v>149</v>
       </c>
@@ -40873,6 +41647,9 @@
       </c>
     </row>
     <row r="260" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A260" s="0" t="n">
+        <v>259</v>
+      </c>
       <c r="B260" s="0" t="s">
         <v>56</v>
       </c>
@@ -40896,6 +41673,9 @@
       </c>
     </row>
     <row r="261" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A261" s="0" t="n">
+        <v>260</v>
+      </c>
       <c r="B261" s="0" t="s">
         <v>737</v>
       </c>
@@ -40919,6 +41699,9 @@
       </c>
     </row>
     <row r="262" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A262" s="0" t="n">
+        <v>261</v>
+      </c>
       <c r="B262" s="0" t="s">
         <v>86</v>
       </c>
@@ -40942,6 +41725,9 @@
       </c>
     </row>
     <row r="263" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A263" s="0" t="n">
+        <v>262</v>
+      </c>
       <c r="B263" s="0" t="s">
         <v>29</v>
       </c>
@@ -40965,6 +41751,9 @@
       </c>
     </row>
     <row r="264" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A264" s="0" t="n">
+        <v>263</v>
+      </c>
       <c r="B264" s="0" t="s">
         <v>118</v>
       </c>
@@ -40988,6 +41777,9 @@
       </c>
     </row>
     <row r="265" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A265" s="0" t="n">
+        <v>264</v>
+      </c>
       <c r="B265" s="0" t="s">
         <v>118</v>
       </c>
@@ -41011,6 +41803,9 @@
       </c>
     </row>
     <row r="266" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A266" s="0" t="n">
+        <v>265</v>
+      </c>
       <c r="B266" s="0" t="s">
         <v>118</v>
       </c>
@@ -41034,6 +41829,9 @@
       </c>
     </row>
     <row r="267" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A267" s="0" t="n">
+        <v>266</v>
+      </c>
       <c r="B267" s="0" t="s">
         <v>9</v>
       </c>
@@ -41057,6 +41855,9 @@
       </c>
     </row>
     <row r="268" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A268" s="0" t="n">
+        <v>267</v>
+      </c>
       <c r="B268" s="0" t="s">
         <v>16</v>
       </c>
@@ -41080,6 +41881,9 @@
       </c>
     </row>
     <row r="269" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A269" s="0" t="n">
+        <v>268</v>
+      </c>
       <c r="B269" s="0" t="s">
         <v>86</v>
       </c>
@@ -41103,6 +41907,9 @@
       </c>
     </row>
     <row r="270" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A270" s="0" t="n">
+        <v>269</v>
+      </c>
       <c r="B270" s="0" t="s">
         <v>86</v>
       </c>
@@ -41126,6 +41933,9 @@
       </c>
     </row>
     <row r="271" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A271" s="0" t="n">
+        <v>270</v>
+      </c>
       <c r="B271" s="0" t="s">
         <v>298</v>
       </c>
@@ -41149,6 +41959,9 @@
       </c>
     </row>
     <row r="272" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A272" s="0" t="n">
+        <v>271</v>
+      </c>
       <c r="B272" s="0" t="s">
         <v>149</v>
       </c>
@@ -41172,6 +41985,9 @@
       </c>
     </row>
     <row r="273" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A273" s="0" t="n">
+        <v>272</v>
+      </c>
       <c r="B273" s="0" t="s">
         <v>86</v>
       </c>
@@ -41195,6 +42011,9 @@
       </c>
     </row>
     <row r="274" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A274" s="0" t="n">
+        <v>273</v>
+      </c>
       <c r="B274" s="0" t="s">
         <v>325</v>
       </c>
@@ -41218,6 +42037,9 @@
       </c>
     </row>
     <row r="275" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A275" s="0" t="n">
+        <v>274</v>
+      </c>
       <c r="B275" s="0" t="s">
         <v>16</v>
       </c>
@@ -41241,6 +42063,9 @@
       </c>
     </row>
     <row r="276" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A276" s="0" t="n">
+        <v>275</v>
+      </c>
       <c r="B276" s="0" t="s">
         <v>86</v>
       </c>
@@ -41264,6 +42089,9 @@
       </c>
     </row>
     <row r="277" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A277" s="0" t="n">
+        <v>276</v>
+      </c>
       <c r="B277" s="0" t="s">
         <v>56</v>
       </c>
@@ -41287,6 +42115,9 @@
       </c>
     </row>
     <row r="278" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A278" s="0" t="n">
+        <v>277</v>
+      </c>
       <c r="B278" s="0" t="s">
         <v>1489</v>
       </c>
@@ -41310,6 +42141,9 @@
       </c>
     </row>
     <row r="279" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A279" s="0" t="n">
+        <v>278</v>
+      </c>
       <c r="B279" s="0" t="s">
         <v>298</v>
       </c>
@@ -41333,6 +42167,9 @@
       </c>
     </row>
     <row r="280" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A280" s="0" t="n">
+        <v>279</v>
+      </c>
       <c r="B280" s="0" t="s">
         <v>298</v>
       </c>
@@ -41356,6 +42193,9 @@
       </c>
     </row>
     <row r="281" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A281" s="0" t="n">
+        <v>280</v>
+      </c>
       <c r="B281" s="0" t="s">
         <v>125</v>
       </c>
@@ -41379,6 +42219,9 @@
       </c>
     </row>
     <row r="282" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A282" s="0" t="n">
+        <v>281</v>
+      </c>
       <c r="B282" s="0" t="s">
         <v>149</v>
       </c>
@@ -41402,6 +42245,9 @@
       </c>
     </row>
     <row r="283" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A283" s="0" t="n">
+        <v>282</v>
+      </c>
       <c r="B283" s="0" t="s">
         <v>325</v>
       </c>
@@ -41425,6 +42271,9 @@
       </c>
     </row>
     <row r="284" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A284" s="0" t="n">
+        <v>283</v>
+      </c>
       <c r="B284" s="0" t="s">
         <v>118</v>
       </c>
@@ -41448,6 +42297,9 @@
       </c>
     </row>
     <row r="285" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A285" s="0" t="n">
+        <v>284</v>
+      </c>
       <c r="B285" s="0" t="s">
         <v>9</v>
       </c>
@@ -41471,6 +42323,9 @@
       </c>
     </row>
     <row r="286" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A286" s="0" t="n">
+        <v>285</v>
+      </c>
       <c r="B286" s="0" t="s">
         <v>118</v>
       </c>
@@ -41494,6 +42349,9 @@
       </c>
     </row>
     <row r="287" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A287" s="0" t="n">
+        <v>286</v>
+      </c>
       <c r="B287" s="0" t="s">
         <v>93</v>
       </c>
@@ -41517,6 +42375,9 @@
       </c>
     </row>
     <row r="288" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A288" s="0" t="n">
+        <v>287</v>
+      </c>
       <c r="B288" s="0" t="s">
         <v>118</v>
       </c>
@@ -41540,6 +42401,9 @@
       </c>
     </row>
     <row r="289" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A289" s="0" t="n">
+        <v>288</v>
+      </c>
       <c r="B289" s="0" t="s">
         <v>118</v>
       </c>
@@ -41563,6 +42427,9 @@
       </c>
     </row>
     <row r="290" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A290" s="0" t="n">
+        <v>289</v>
+      </c>
       <c r="B290" s="0" t="s">
         <v>464</v>
       </c>
@@ -41586,6 +42453,9 @@
       </c>
     </row>
     <row r="291" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A291" s="0" t="n">
+        <v>290</v>
+      </c>
       <c r="B291" s="0" t="s">
         <v>149</v>
       </c>
@@ -41609,6 +42479,9 @@
       </c>
     </row>
     <row r="292" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A292" s="0" t="n">
+        <v>291</v>
+      </c>
       <c r="B292" s="0" t="s">
         <v>118</v>
       </c>
@@ -41632,6 +42505,9 @@
       </c>
     </row>
     <row r="293" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A293" s="0" t="n">
+        <v>292</v>
+      </c>
       <c r="B293" s="0" t="s">
         <v>464</v>
       </c>
@@ -41655,6 +42531,9 @@
       </c>
     </row>
     <row r="294" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A294" s="0" t="n">
+        <v>293</v>
+      </c>
       <c r="B294" s="0" t="s">
         <v>737</v>
       </c>
@@ -41678,6 +42557,9 @@
       </c>
     </row>
     <row r="295" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A295" s="0" t="n">
+        <v>294</v>
+      </c>
       <c r="B295" s="0" t="s">
         <v>737</v>
       </c>
@@ -41701,6 +42583,9 @@
       </c>
     </row>
     <row r="296" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A296" s="0" t="n">
+        <v>295</v>
+      </c>
       <c r="B296" s="0" t="s">
         <v>125</v>
       </c>
@@ -41724,6 +42609,9 @@
       </c>
     </row>
     <row r="297" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A297" s="0" t="n">
+        <v>296</v>
+      </c>
       <c r="B297" s="0" t="s">
         <v>149</v>
       </c>
@@ -41747,6 +42635,9 @@
       </c>
     </row>
     <row r="298" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A298" s="0" t="n">
+        <v>297</v>
+      </c>
       <c r="B298" s="0" t="s">
         <v>149</v>
       </c>
@@ -41770,6 +42661,9 @@
       </c>
     </row>
     <row r="299" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A299" s="0" t="n">
+        <v>298</v>
+      </c>
       <c r="B299" s="0" t="s">
         <v>162</v>
       </c>
@@ -41793,6 +42687,9 @@
       </c>
     </row>
     <row r="300" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A300" s="0" t="n">
+        <v>299</v>
+      </c>
       <c r="B300" s="0" t="s">
         <v>464</v>
       </c>
@@ -41816,6 +42713,9 @@
       </c>
     </row>
     <row r="301" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A301" s="0" t="n">
+        <v>300</v>
+      </c>
       <c r="B301" s="0" t="s">
         <v>149</v>
       </c>
@@ -41839,6 +42739,9 @@
       </c>
     </row>
     <row r="302" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A302" s="0" t="n">
+        <v>301</v>
+      </c>
       <c r="B302" s="0" t="s">
         <v>118</v>
       </c>
@@ -41862,6 +42765,9 @@
       </c>
     </row>
     <row r="303" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A303" s="0" t="n">
+        <v>302</v>
+      </c>
       <c r="B303" s="0" t="s">
         <v>298</v>
       </c>
@@ -41885,6 +42791,9 @@
       </c>
     </row>
     <row r="304" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A304" s="0" t="n">
+        <v>303</v>
+      </c>
       <c r="B304" s="0" t="s">
         <v>125</v>
       </c>
@@ -41908,6 +42817,9 @@
       </c>
     </row>
     <row r="305" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A305" s="0" t="n">
+        <v>304</v>
+      </c>
       <c r="B305" s="0" t="s">
         <v>9</v>
       </c>
@@ -41931,6 +42843,9 @@
       </c>
     </row>
     <row r="306" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A306" s="0" t="n">
+        <v>305</v>
+      </c>
       <c r="B306" s="0" t="s">
         <v>125</v>
       </c>
@@ -41954,6 +42869,9 @@
       </c>
     </row>
     <row r="307" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A307" s="0" t="n">
+        <v>306</v>
+      </c>
       <c r="B307" s="0" t="s">
         <v>936</v>
       </c>
@@ -41977,6 +42895,9 @@
       </c>
     </row>
     <row r="308" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A308" s="0" t="n">
+        <v>307</v>
+      </c>
       <c r="B308" s="0" t="s">
         <v>29</v>
       </c>

</xml_diff>